<commit_message>
get sheet name and year + test
</commit_message>
<xml_diff>
--- a/files/test-input.xlsx
+++ b/files/test-input.xlsx
@@ -5,14 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="LIT" sheetId="1" r:id="rId4"/>
-    <sheet name="GRAMMAR" sheetId="2" r:id="rId5"/>
+    <sheet name="Lit 3 2019-2020" sheetId="1" r:id="rId4"/>
+    <sheet name="Grammar 4 2019-2020" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -20,13 +20,37 @@
     <t>Last name</t>
   </si>
   <si>
-    <t>Retake</t>
-  </si>
-  <si>
     <t>Mark</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>Isa</t>
+  </si>
+  <si>
+    <t>Garvi</t>
+  </si>
+  <si>
+    <t>Cris</t>
+  </si>
+  <si>
+    <t>Rodero</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Alejandra</t>
+  </si>
+  <si>
+    <t>Carretero</t>
+  </si>
+  <si>
+    <t>Nela</t>
+  </si>
+  <si>
+    <t>Alberola</t>
   </si>
   <si>
     <t>Cdddv</t>
@@ -216,7 +240,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -226,13 +250,22 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -245,6 +278,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1330,14 +1372,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1350,159 +1392,141 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="B2" t="s" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -1524,89 +1548,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="9" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
docstrings on excel file processor and more custom errors
</commit_message>
<xml_diff>
--- a/files/test-input.xlsx
+++ b/files/test-input.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -51,18 +51,6 @@
   </si>
   <si>
     <t>Alberola</t>
-  </si>
-  <si>
-    <t>Cdddv</t>
-  </si>
-  <si>
-    <t>Dvddv</t>
-  </si>
-  <si>
-    <t>Dvddvv</t>
-  </si>
-  <si>
-    <t>Vsdvsdv</t>
   </si>
 </sst>
 </file>
@@ -116,12 +104,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -148,6 +136,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
@@ -193,6 +203,24 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
@@ -234,13 +262,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -250,43 +300,61 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -309,8 +377,9 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1372,14 +1441,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1392,141 +1461,185 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="7">
         <v>9</v>
       </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="12">
         <v>8</v>
       </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="11">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="12">
         <v>3</v>
       </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="12">
         <v>2</v>
       </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="10">
         <v>11</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="12">
         <v>7</v>
       </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -1542,95 +1655,71 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>